<commit_message>
Update parameter file to allow usage of specific atlas files
</commit_message>
<xml_diff>
--- a/ClearMap/Scripts/batch processing/variable_file.xlsx
+++ b/ClearMap/Scripts/batch processing/variable_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuberadmin\Desktop\SHIELD\ClearMap related files\ClearMap\ClearMap_ForHPC_UW\ClearMap\Scripts\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuberadmin\Desktop\SHIELD\ClearMap related files\ClearMap\ClearMap_ForHPC_UW\ClearMap\Scripts\batch processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D5701A-E37E-4DD2-A8D1-B9D878597E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF10637-45AA-4F68-BD5A-BC1F60CACD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="2910" windowWidth="21855" windowHeight="11250" tabRatio="752" firstSheet="3" activeTab="5" xr2:uid="{61B71D1B-A7AC-47B3-A961-00FCE0D70380}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="752" activeTab="1" xr2:uid="{61B71D1B-A7AC-47B3-A961-00FCE0D70380}"/>
   </bookViews>
   <sheets>
     <sheet name="CropGeneratingParameter" sheetId="6" r:id="rId1"/>
@@ -42,8 +42,28 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B07D04BA-C91E-4E60-BF84-75E1C2371E8A}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{B07D04BA-C91E-4E60-BF84-75E1C2371E8A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    "YK" for Kim unified
+"Allen" for CCFv3
+"Rat" for Waxholm atlas</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>AtlasResolution</t>
   </si>
@@ -214,13 +234,19 @@
   </si>
   <si>
     <t>(80,)</t>
+  </si>
+  <si>
+    <t>Atlas_name</t>
+  </si>
+  <si>
+    <t>YK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +257,12 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -286,6 +318,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="ken1223" id="{1A5E9F5D-5DBE-419E-B8B2-020EAA6CC949}" userId="S::ken1223@uw.edu::8aae8380-cb34-4c98-88c8-6f9ae900ba4e" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -603,6 +641,16 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2024-06-13T21:59:10.68" personId="{1A5E9F5D-5DBE-419E-B8B2-020EAA6CC949}" id="{B07D04BA-C91E-4E60-BF84-75E1C2371E8A}">
+    <text>"YK" for Kim unified
+"Allen" for CCFv3
+"Rat" for Waxholm atlas</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43DA83E-D86A-429D-9597-C6C832EFE925}">
   <dimension ref="A1:G2"/>
@@ -670,60 +718,68 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAD0F49-F2B1-4086-BF5B-BDC00B76680F}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAD0F49-F2B1-4086-BF5B-BDC00B76680F}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -854,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06822A0D-C61A-464F-9B81-3D4B494EBE81}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>

</xml_diff>